<commit_message>
FIxed orders excel and added some error handlings
</commit_message>
<xml_diff>
--- a/resources/imports/orders.xlsx
+++ b/resources/imports/orders.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28422"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktor\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E4ABCD-073E-4EFE-ABE0-65DA4066C045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="13320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t>Order date</t>
   </si>
@@ -62,6 +56,9 @@
     <t>Total Price</t>
   </si>
   <si>
+    <t>01-12-2024</t>
+  </si>
+  <si>
     <t>Amazon</t>
   </si>
   <si>
@@ -77,6 +74,9 @@
     <t>SO1001</t>
   </si>
   <si>
+    <t>02-12-2024</t>
+  </si>
+  <si>
     <t>SKU67890</t>
   </si>
   <si>
@@ -89,6 +89,9 @@
     <t>SO1002</t>
   </si>
   <si>
+    <t>03-12-2024</t>
+  </si>
+  <si>
     <t>SKU23456</t>
   </si>
   <si>
@@ -101,6 +104,9 @@
     <t>SO1003</t>
   </si>
   <si>
+    <t>04-12-2024</t>
+  </si>
+  <si>
     <t>PT</t>
   </si>
   <si>
@@ -113,6 +119,9 @@
     <t>SO1004</t>
   </si>
   <si>
+    <t>05-12-2024</t>
+  </si>
+  <si>
     <t>SKU34567</t>
   </si>
   <si>
@@ -125,6 +134,9 @@
     <t>SO1005</t>
   </si>
   <si>
+    <t>06-12-2024</t>
+  </si>
+  <si>
     <t>SKU45678</t>
   </si>
   <si>
@@ -134,6 +146,9 @@
     <t>SO1006</t>
   </si>
   <si>
+    <t>07-12-2024</t>
+  </si>
+  <si>
     <t>SKU56789</t>
   </si>
   <si>
@@ -143,6 +158,9 @@
     <t>SO1007</t>
   </si>
   <si>
+    <t>08-12-2024</t>
+  </si>
+  <si>
     <t>SKU67801</t>
   </si>
   <si>
@@ -152,6 +170,9 @@
     <t>SO1008</t>
   </si>
   <si>
+    <t>09-12-2024</t>
+  </si>
+  <si>
     <t>SKU78912</t>
   </si>
   <si>
@@ -164,6 +185,9 @@
     <t>SO1009</t>
   </si>
   <si>
+    <t>10-12-2024</t>
+  </si>
+  <si>
     <t>SKU89013</t>
   </si>
   <si>
@@ -171,46 +195,20 @@
   </si>
   <si>
     <t>SO1010</t>
-  </si>
-  <si>
-    <t>01-12-2024</t>
-  </si>
-  <si>
-    <t>02-12-2024</t>
-  </si>
-  <si>
-    <t>03-12-2024</t>
-  </si>
-  <si>
-    <t>04-12-2024</t>
-  </si>
-  <si>
-    <t>05-12-2024</t>
-  </si>
-  <si>
-    <t>06-12-2024</t>
-  </si>
-  <si>
-    <t>07-12-2024</t>
-  </si>
-  <si>
-    <t>08-12-2024</t>
-  </si>
-  <si>
-    <t>09-12-2024</t>
-  </si>
-  <si>
-    <t>10-12-2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,18 +220,348 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -241,9 +569,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -254,21 +824,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -546,32 +1160,32 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.4416666666667" customWidth="1"/>
+    <col min="2" max="2" width="26.1083333333333" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.5583333333333" customWidth="1"/>
+    <col min="5" max="5" width="14.5583333333333" customWidth="1"/>
+    <col min="6" max="6" width="11.1083333333333" customWidth="1"/>
+    <col min="7" max="7" width="13.8833333333333" customWidth="1"/>
+    <col min="8" max="8" width="15.1083333333333" customWidth="1"/>
+    <col min="9" max="9" width="12.5583333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,24 +1214,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3">
         <v>15</v>
@@ -629,24 +1243,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3">
         <v>25</v>
@@ -658,24 +1272,24 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3">
         <v>30</v>
@@ -687,22 +1301,24 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" ht="34.2" customHeight="1" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="F5" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G5" s="3">
         <v>50</v>
@@ -714,24 +1330,24 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G6" s="3">
         <v>12</v>
@@ -743,24 +1359,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G7" s="3">
         <v>100</v>
@@ -772,24 +1388,24 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G8" s="3">
         <v>20</v>
@@ -801,24 +1417,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="G9" s="3">
         <v>40</v>
@@ -830,24 +1446,24 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G10" s="3">
         <v>22</v>
@@ -859,24 +1475,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="G11" s="3">
         <v>8</v>
@@ -890,5 +1506,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>